<commit_message>
Virginia model updated Investment Cost projections starting in 2025 and changing over time based on NREL ATB Refined limits for natural gas and biomass consumption
</commit_message>
<xml_diff>
--- a/projects/va_emerging_tech/data/scenarios_emerging_tech.xlsx
+++ b/projects/va_emerging_tech/data/scenarios_emerging_tech.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DDB7D5-7755-46D8-84B9-4AB3EB7984E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4783B8-AB98-4542-B6C4-1C42A3ACA60C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="95">
   <si>
     <t>Scenario</t>
   </si>
@@ -396,9 +396,6 @@
     <t>E_BECCS</t>
   </si>
   <si>
-    <t>BIO_TO_ATM</t>
-  </si>
-  <si>
     <t>BIO_TO_CCS</t>
   </si>
   <si>
@@ -412,12 +409,6 @@
   </si>
   <si>
     <t>E_PV_DIST_RES</t>
-  </si>
-  <si>
-    <t>BAU</t>
-  </si>
-  <si>
-    <t>unconstrained</t>
   </si>
   <si>
     <r>
@@ -994,7 +985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E4BDBC8-04C0-4C73-8BBF-CE8A7DD9E8F0}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1061,13 +1052,13 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -1150,48 +1141,42 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="13.88671875" customWidth="1"/>
+    <col min="2" max="7" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1213,14 +1198,8 @@
       <c r="G2" t="s">
         <v>28</v>
       </c>
-      <c r="H2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1242,14 +1221,8 @@
       <c r="G3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1271,14 +1244,8 @@
       <c r="G4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1300,14 +1267,8 @@
       <c r="G5">
         <v>30</v>
       </c>
-      <c r="H5">
-        <v>30</v>
-      </c>
-      <c r="I5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1329,22 +1290,16 @@
       <c r="G6" t="s">
         <v>28</v>
       </c>
-      <c r="H6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
         <v>17</v>
@@ -1358,16 +1313,10 @@
       <c r="G7" t="s">
         <v>17</v>
       </c>
-      <c r="H7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
         <v>28</v>
@@ -1387,14 +1336,8 @@
       <c r="G8" t="s">
         <v>28</v>
       </c>
-      <c r="H8" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>27</v>
       </c>
@@ -1416,14 +1359,8 @@
       <c r="G9" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>29</v>
       </c>
@@ -1445,14 +1382,8 @@
       <c r="G10" s="14">
         <v>20</v>
       </c>
-      <c r="H10" s="14">
-        <v>20</v>
-      </c>
-      <c r="I10" s="14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>30</v>
       </c>
@@ -1474,40 +1405,34 @@
       <c r="G11" s="14">
         <v>1000</v>
       </c>
-      <c r="H11" s="14">
-        <v>1000</v>
-      </c>
-      <c r="I11" s="14">
-        <v>1000</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:C9 J2:XFD9 E2:E9">
+  <conditionalFormatting sqref="H2:XFD9 C2:C9">
     <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F9">
+  <conditionalFormatting sqref="D2:D9">
     <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G9">
+  <conditionalFormatting sqref="E2:E9">
     <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H9">
+  <conditionalFormatting sqref="F2:F9">
     <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I9">
+  <conditionalFormatting sqref="G2:G9">
     <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D9">
+  <conditionalFormatting sqref="B2:B9">
     <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -1519,48 +1444,42 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" activeCellId="1" sqref="B1:B1048576 C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="13.88671875" customWidth="1"/>
+    <col min="2" max="7" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1582,16 +1501,10 @@
       <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>17</v>
@@ -1611,14 +1524,8 @@
       <c r="G3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1640,14 +1547,8 @@
       <c r="G4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1669,16 +1570,10 @@
       <c r="G5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>17</v>
@@ -1698,14 +1593,8 @@
       <c r="G6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1727,14 +1616,8 @@
       <c r="G7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1756,14 +1639,8 @@
       <c r="G8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1785,16 +1662,10 @@
       <c r="G9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>95</v>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>17</v>
@@ -1814,15 +1685,9 @@
       <c r="G10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1843,15 +1708,9 @@
       <c r="G11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1872,15 +1731,9 @@
       <c r="G12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1901,43 +1754,19 @@
       <c r="G13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1959,14 +1788,8 @@
       <c r="G15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -1988,14 +1811,8 @@
       <c r="G16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -2017,14 +1834,8 @@
       <c r="G17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -2046,14 +1857,8 @@
       <c r="G18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -2075,14 +1880,8 @@
       <c r="G19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -2104,14 +1903,8 @@
       <c r="G20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -2133,14 +1926,8 @@
       <c r="G21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -2162,16 +1949,10 @@
       <c r="G22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>17</v>
@@ -2191,49 +1972,36 @@
       <c r="G23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D24" s="1"/>
-      <c r="E24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G24" s="1"/>
-      <c r="H24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>
       </c>
-      <c r="E25" t="s">
-        <v>17</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G25" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C26" t="s">
         <v>17</v>
@@ -2241,11 +2009,8 @@
       <c r="E26" t="s">
         <v>17</v>
       </c>
-      <c r="G26" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>68</v>
       </c>
@@ -2267,14 +2032,8 @@
       <c r="G27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>69</v>
       </c>
@@ -2282,29 +2041,25 @@
       <c r="C28" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="D28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:C1048576 E2:XFD1048576">
+  <conditionalFormatting sqref="C2:XFD1048576">
     <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D24:D1048576">
+  <conditionalFormatting sqref="B24:B1048576">
     <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D23">
+  <conditionalFormatting sqref="B2:B23">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2316,48 +2071,42 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C1" activeCellId="1" sqref="B1:B1048576 C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="13.88671875" customWidth="1"/>
+    <col min="2" max="7" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -2379,14 +2128,8 @@
       <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -2408,14 +2151,8 @@
       <c r="G3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -2437,14 +2174,8 @@
       <c r="G4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -2466,14 +2197,8 @@
       <c r="G5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -2495,14 +2220,8 @@
       <c r="G6" t="s">
         <v>17</v>
       </c>
-      <c r="H6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -2524,14 +2243,8 @@
       <c r="G7" t="s">
         <v>17</v>
       </c>
-      <c r="H7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
@@ -2553,14 +2266,8 @@
       <c r="G8" t="s">
         <v>17</v>
       </c>
-      <c r="H8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -2582,30 +2289,24 @@
       <c r="G9" t="s">
         <v>17</v>
       </c>
-      <c r="H9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" t="s">
-        <v>17</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B10:XFD1048576 B3:C9 E3:XFD9 J2:XFD2">
+  <conditionalFormatting sqref="C3:XFD9 H2:XFD2 B10:XFD1048576">
     <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D9">
+  <conditionalFormatting sqref="B3:B9">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:C2 E2:I2">
+  <conditionalFormatting sqref="C2:G2">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="B2">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -2616,48 +2317,42 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:I15"/>
+      <selection activeCell="C1" activeCellId="1" sqref="B1:B1048576 C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="13.88671875" customWidth="1"/>
+    <col min="2" max="7" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -2679,14 +2374,8 @@
       <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -2708,14 +2397,8 @@
       <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -2737,14 +2420,8 @@
       <c r="G4" t="s">
         <v>17</v>
       </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -2766,14 +2443,8 @@
       <c r="G5" t="s">
         <v>17</v>
       </c>
-      <c r="H5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2795,100 +2466,82 @@
       <c r="G6" t="s">
         <v>17</v>
       </c>
-      <c r="H6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>87</v>
-      </c>
       <c r="B14" t="s">
         <v>17</v>
       </c>
@@ -2907,16 +2560,10 @@
       <c r="G14" t="s">
         <v>17</v>
       </c>
-      <c r="H14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B15" t="s">
         <v>17</v>
@@ -2936,67 +2583,26 @@
       <c r="G15" t="s">
         <v>17</v>
       </c>
-      <c r="H15" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
       </c>
-      <c r="E16" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>70</v>
       </c>
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
       <c r="C17" t="s">
         <v>17</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>71</v>
-      </c>
-      <c r="C18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>